<commit_message>
atualização e funcionando perfeitamente agora para o modo ESCURO DO WHATSZAPP WEB
</commit_message>
<xml_diff>
--- a/contatos/clientes.xlsx
+++ b/contatos/clientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DocumentosHD\bot whatsapp\contatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06A0021-45B5-4081-BF88-638EEE8FCDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33F2BE8-B96C-4675-8FE0-EC9564DC0034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11670" yWindow="2940" windowWidth="13890" windowHeight="10635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pagina1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>nome</t>
   </si>
@@ -37,6 +37,42 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>55 61 9904-9373</t>
+  </si>
+  <si>
+    <t>produto</t>
+  </si>
+  <si>
+    <t>Caneca - Tirante - Camisa Oversized Branca - Camisa Oversized Preta  - Regata Azul</t>
+  </si>
+  <si>
+    <t>Beatriz lima</t>
+  </si>
+  <si>
+    <t>55 61 8282-7605</t>
+  </si>
+  <si>
+    <t>Caneca - Tirante - body</t>
+  </si>
+  <si>
+    <t>55 61 9235-4323</t>
+  </si>
+  <si>
+    <t>Yan Flu</t>
+  </si>
+  <si>
+    <t>Samba - Caneca - Tirante</t>
+  </si>
+  <si>
+    <t>Moreira</t>
+  </si>
+  <si>
+    <t>55 61 8659-4667</t>
+  </si>
+  <si>
+    <t>Camisa Oversized Preta - Caneca e Tirante</t>
   </si>
 </sst>
 </file>
@@ -46,15 +82,8 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -81,16 +110,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,48 +403,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
-        <v>5561000000000</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="4"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C4" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C7" s="6"/>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45607</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45607</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45607</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45607</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
ajustes no README.md e apagamento dos dados da planilha
</commit_message>
<xml_diff>
--- a/contatos/clientes.xlsx
+++ b/contatos/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DocumentosHD\bot whatsapp\contatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33F2BE8-B96C-4675-8FE0-EC9564DC0034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA36902-A2EC-43AB-898B-F798A43E46B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11670" yWindow="2940" windowWidth="13890" windowHeight="10635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>nome</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Good</t>
   </si>
   <si>
-    <t>55 61 9904-9373</t>
-  </si>
-  <si>
     <t>produto</t>
   </si>
   <si>
@@ -51,15 +48,9 @@
     <t>Beatriz lima</t>
   </si>
   <si>
-    <t>55 61 8282-7605</t>
-  </si>
-  <si>
     <t>Caneca - Tirante - body</t>
   </si>
   <si>
-    <t>55 61 9235-4323</t>
-  </si>
-  <si>
     <t>Yan Flu</t>
   </si>
   <si>
@@ -69,10 +60,10 @@
     <t>Moreira</t>
   </si>
   <si>
-    <t>55 61 8659-4667</t>
-  </si>
-  <si>
     <t>Camisa Oversized Preta - Caneca e Tirante</t>
+  </si>
+  <si>
+    <t>55 00 0000-0000</t>
   </si>
 </sst>
 </file>
@@ -110,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -118,9 +109,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -403,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -426,7 +414,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -434,59 +422,56 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>45607</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>45607</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>45607</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>45607</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>